<commit_message>
Update randomization procedure for sample table
</commit_message>
<xml_diff>
--- a/part_10-working_with_tables_files/plate_1.xlsx
+++ b/part_10-working_with_tables_files/plate_1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Benjamin/Documents/University/1712-2011 PhD/PhD_Thesis/_sync/octo_waffle/part_10-working_with_tables_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0E307527-B528-CB47-85CD-0026E08A112B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D919CDB8-C7F9-9141-9C86-2105EBCAF52E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="1800" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="10360" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plate_1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -536,8 +539,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -892,11 +896,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -925,20 +929,20 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
-        <v>1.6E-2</v>
-      </c>
-      <c r="E4">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="F4">
-        <v>-0.307</v>
-      </c>
-      <c r="G4">
-        <v>-2E-3</v>
-      </c>
-      <c r="H4">
-        <v>7.0000000000000001E-3</v>
+      <c r="D4" s="1">
+        <v>-0.98599999999999999</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-0.377</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-0.16500000000000001</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-0.40200000000000002</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
@@ -948,20 +952,20 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="E5">
-        <v>-6.3E-2</v>
-      </c>
-      <c r="F5">
-        <v>0.30099999999999999</v>
-      </c>
-      <c r="G5">
-        <v>0.15</v>
-      </c>
-      <c r="H5">
-        <v>-0.70399999999999996</v>
+      <c r="D5" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
@@ -971,20 +975,20 @@
       <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
-        <v>6.4770000000000003</v>
-      </c>
-      <c r="E6">
-        <v>3.839</v>
-      </c>
-      <c r="F6">
-        <v>3.0640000000000001</v>
-      </c>
-      <c r="G6">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="H6">
-        <v>0.182</v>
+      <c r="D6" s="1">
+        <v>5.992</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4.7110000000000003</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2.504</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="H6" s="1">
+        <v>-0.21099999999999999</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
@@ -994,20 +998,20 @@
       <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
-        <v>5.7549999999999999</v>
-      </c>
-      <c r="E7">
-        <v>3.7280000000000002</v>
-      </c>
-      <c r="F7">
-        <v>2.153</v>
-      </c>
-      <c r="G7">
-        <v>-0.08</v>
-      </c>
-      <c r="H7">
-        <v>0.20399999999999999</v>
+      <c r="D7" s="1">
+        <v>6.5209999999999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3.5739999999999998</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.7569999999999999</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1.482</v>
+      </c>
+      <c r="H7" s="1">
+        <v>8.1000000000000003E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>